<commit_message>
re-generated as bar chart
</commit_message>
<xml_diff>
--- a/results/StatesThroughTime-bin50.xlsx
+++ b/results/StatesThroughTime-bin50.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="12920" yWindow="4680" windowWidth="25360" windowHeight="18780" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Grafiek1" sheetId="2" r:id="rId1"/>
@@ -62,7 +62,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="129"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -90,7 +89,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normaal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -113,7 +112,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="nl-NL"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -127,7 +126,8 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:areaChart>
+      <c:barChart>
+        <c:barDir val="col"/>
         <c:grouping val="percentStacked"/>
         <c:varyColors val="0"/>
         <c:ser>
@@ -144,6 +144,7 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>'StatesThroughTime-bin50.txt'!$A$2:$A$12</c:f>
@@ -243,6 +244,7 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>'StatesThroughTime-bin50.txt'!$A$2:$A$12</c:f>
@@ -342,6 +344,7 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>'StatesThroughTime-bin50.txt'!$A$2:$A$12</c:f>
@@ -441,6 +444,7 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>'StatesThroughTime-bin50.txt'!$A$2:$A$12</c:f>
@@ -540,6 +544,7 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>'StatesThroughTime-bin50.txt'!$A$2:$A$12</c:f>
@@ -639,6 +644,7 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>'StatesThroughTime-bin50.txt'!$A$2:$A$12</c:f>
@@ -738,6 +744,7 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>'StatesThroughTime-bin50.txt'!$A$2:$A$12</c:f>
@@ -837,6 +844,7 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>'StatesThroughTime-bin50.txt'!$A$2:$A$12</c:f>
@@ -936,6 +944,7 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>'StatesThroughTime-bin50.txt'!$A$2:$A$12</c:f>
@@ -1029,11 +1038,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2102068808"/>
-        <c:axId val="-2101461512"/>
-      </c:areaChart>
+        <c:gapWidth val="0"/>
+        <c:overlap val="100"/>
+        <c:axId val="408440808"/>
+        <c:axId val="408443752"/>
+      </c:barChart>
       <c:catAx>
-        <c:axId val="-2102068808"/>
+        <c:axId val="408440808"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1052,10 +1063,10 @@
                 <a:latin typeface="Verdana"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="nl-NL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2101461512"/>
+        <c:crossAx val="408443752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1063,21 +1074,26 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2101461512"/>
+        <c:axId val="408443752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="r"/>
-        <c:majorGridlines/>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2102068808"/>
+        <c:crossAx val="408440808"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
@@ -1092,7 +1108,7 @@
               <a:latin typeface="Verdana"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="nl-NL"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1107,7 +1123,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="163" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="127" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1119,7 +1135,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9201656" cy="5609816"/>
+    <xdr:ext cx="9210000" cy="5620000"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Grafiek 1"/>

</xml_diff>